<commit_message>
bugfix: IsGroupStageFinished checks wrong excel sheet. + result logging
</commit_message>
<xml_diff>
--- a/bin/Debug/_Fasit/Fasit.xlsx
+++ b/bin/Debug/_Fasit/Fasit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hallstein\SkyDrive\DEV\Euro2016\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hallstein\SkyDrive\DEV\EM2016\bin\Debug\_Fasit\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29133,8 +29133,8 @@
   </sheetPr>
   <dimension ref="A1:DY97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="DW36" sqref="DW36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.09765625" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -30771,9 +30771,7 @@
         <f>BC9</f>
         <v>Sveits</v>
       </c>
-      <c r="DF10" s="61">
-        <v>2</v>
-      </c>
+      <c r="DF10" s="61"/>
       <c r="DG10" s="126"/>
       <c r="DH10" s="83"/>
       <c r="DI10" s="83"/>
@@ -31157,9 +31155,7 @@
         <f>BC21</f>
         <v>Polen</v>
       </c>
-      <c r="DF11" s="59">
-        <v>1</v>
-      </c>
+      <c r="DF11" s="59"/>
       <c r="DG11" s="127"/>
       <c r="DH11" s="86"/>
       <c r="DI11" s="83"/>
@@ -31448,11 +31444,9 @@
       </c>
       <c r="DK12" s="90" t="str">
         <f>W46</f>
-        <v>Sveits</v>
-      </c>
-      <c r="DL12" s="61">
-        <v>1</v>
-      </c>
+        <v>V37</v>
+      </c>
+      <c r="DL12" s="61"/>
       <c r="DM12" s="126"/>
       <c r="DN12" s="83"/>
       <c r="DO12" s="83"/>
@@ -31608,11 +31602,9 @@
       <c r="DJ13" s="137"/>
       <c r="DK13" s="91" t="str">
         <f>W47</f>
-        <v>Spania</v>
-      </c>
-      <c r="DL13" s="59">
-        <v>2</v>
-      </c>
+        <v>V39</v>
+      </c>
+      <c r="DL13" s="59"/>
       <c r="DM13" s="127"/>
       <c r="DN13" s="86"/>
       <c r="DO13" s="83"/>
@@ -31992,9 +31984,7 @@
         <f>BC26</f>
         <v>Spania</v>
       </c>
-      <c r="DF14" s="61">
-        <v>2</v>
-      </c>
+      <c r="DF14" s="61"/>
       <c r="DG14" s="126"/>
       <c r="DH14" s="87"/>
       <c r="DI14" s="83"/>
@@ -32378,9 +32368,7 @@
         <f>VLOOKUP(lookup_3rd, tbl_lookup_3rd,5,FALSE)</f>
         <v>Sverige</v>
       </c>
-      <c r="DF15" s="59">
-        <v>0</v>
-      </c>
+      <c r="DF15" s="59"/>
       <c r="DG15" s="127"/>
       <c r="DH15" s="83"/>
       <c r="DI15" s="83"/>
@@ -32482,15 +32470,15 @@
       </c>
       <c r="X16" s="117">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y16" s="116">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="116">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA16" s="116">
         <f t="shared" si="5"/>
@@ -32779,14 +32767,10 @@
       </c>
       <c r="DQ16" s="90" t="str">
         <f>W57</f>
-        <v>Spania</v>
-      </c>
-      <c r="DR16" s="61">
-        <v>1</v>
-      </c>
-      <c r="DS16" s="126">
-        <v>5</v>
-      </c>
+        <v>V45</v>
+      </c>
+      <c r="DR16" s="61"/>
+      <c r="DS16" s="126"/>
       <c r="DT16" s="83"/>
       <c r="DU16" s="88"/>
       <c r="DV16" s="83"/>
@@ -33166,14 +33150,10 @@
       <c r="DP17" s="137"/>
       <c r="DQ17" s="91" t="str">
         <f>W58</f>
-        <v>Italia</v>
-      </c>
-      <c r="DR17" s="59">
-        <v>1</v>
-      </c>
-      <c r="DS17" s="127">
-        <v>6</v>
-      </c>
+        <v>V46</v>
+      </c>
+      <c r="DR17" s="59"/>
+      <c r="DS17" s="127"/>
       <c r="DT17" s="86"/>
       <c r="DU17" s="89"/>
       <c r="DV17" s="83"/>
@@ -33442,9 +33422,7 @@
         <f>BC14</f>
         <v>England</v>
       </c>
-      <c r="DF18" s="61">
-        <v>3</v>
-      </c>
+      <c r="DF18" s="61"/>
       <c r="DG18" s="126"/>
       <c r="DH18" s="83"/>
       <c r="DI18" s="83"/>
@@ -33599,9 +33577,7 @@
         <f>VLOOKUP(lookup_3rd, tbl_lookup_3rd,3,FALSE)</f>
         <v>Romania</v>
       </c>
-      <c r="DF19" s="59">
-        <v>1</v>
-      </c>
+      <c r="DF19" s="59"/>
       <c r="DG19" s="127"/>
       <c r="DH19" s="86"/>
       <c r="DI19" s="83"/>
@@ -33994,11 +33970,9 @@
       </c>
       <c r="DK20" s="90" t="str">
         <f>W50</f>
-        <v>England</v>
-      </c>
-      <c r="DL20" s="61">
-        <v>1</v>
-      </c>
+        <v>V38</v>
+      </c>
+      <c r="DL20" s="61"/>
       <c r="DM20" s="126"/>
       <c r="DN20" s="87"/>
       <c r="DO20" s="83"/>
@@ -34383,11 +34357,9 @@
       <c r="DJ21" s="137"/>
       <c r="DK21" s="91" t="str">
         <f>W51</f>
-        <v>Italia</v>
-      </c>
-      <c r="DL21" s="59">
-        <v>2</v>
-      </c>
+        <v>V42</v>
+      </c>
+      <c r="DL21" s="59"/>
       <c r="DM21" s="127"/>
       <c r="DN21" s="83"/>
       <c r="DO21" s="83"/>
@@ -34767,9 +34739,7 @@
         <f>BC38</f>
         <v>Portugal</v>
       </c>
-      <c r="DF22" s="61">
-        <v>0</v>
-      </c>
+      <c r="DF22" s="61"/>
       <c r="DG22" s="126"/>
       <c r="DH22" s="87"/>
       <c r="DI22" s="83"/>
@@ -35150,11 +35120,9 @@
       <c r="DD23" s="139"/>
       <c r="DE23" s="91" t="str">
         <f>BC33</f>
-        <v>Italia</v>
-      </c>
-      <c r="DF23" s="59">
-        <v>1</v>
-      </c>
+        <v>2E</v>
+      </c>
+      <c r="DF23" s="59"/>
       <c r="DG23" s="127"/>
       <c r="DH23" s="83"/>
       <c r="DI23" s="83"/>
@@ -35175,11 +35143,9 @@
       </c>
       <c r="DW23" s="90" t="str">
         <f>W64</f>
-        <v>Italia</v>
-      </c>
-      <c r="DX23" s="61">
-        <v>0</v>
-      </c>
+        <v>V49</v>
+      </c>
+      <c r="DX23" s="61"/>
       <c r="DY23" s="126"/>
     </row>
     <row r="24" spans="1:129" x14ac:dyDescent="0.3">
@@ -35456,11 +35422,9 @@
       <c r="DV24" s="137"/>
       <c r="DW24" s="91" t="str">
         <f>W65</f>
-        <v>Tyskland</v>
-      </c>
-      <c r="DX24" s="59">
-        <v>2</v>
-      </c>
+        <v>V50</v>
+      </c>
+      <c r="DX24" s="59"/>
       <c r="DY24" s="127"/>
     </row>
     <row r="25" spans="1:129" x14ac:dyDescent="0.3">
@@ -35983,9 +35947,7 @@
         <f>BC20</f>
         <v>Tyskland</v>
       </c>
-      <c r="DF26" s="61">
-        <v>3</v>
-      </c>
+      <c r="DF26" s="61"/>
       <c r="DG26" s="126"/>
       <c r="DH26" s="83"/>
       <c r="DI26" s="83"/>
@@ -36369,9 +36331,7 @@
         <f>VLOOKUP(lookup_3rd, tbl_lookup_3rd,4,FALSE)</f>
         <v>Østerrike</v>
       </c>
-      <c r="DF27" s="59">
-        <v>1</v>
-      </c>
+      <c r="DF27" s="59"/>
       <c r="DG27" s="127"/>
       <c r="DH27" s="86"/>
       <c r="DI27" s="83"/>
@@ -36764,11 +36724,9 @@
       </c>
       <c r="DK28" s="90" t="str">
         <f>W48</f>
-        <v>Tyskland</v>
-      </c>
-      <c r="DL28" s="61">
-        <v>2</v>
-      </c>
+        <v>V41</v>
+      </c>
+      <c r="DL28" s="61"/>
       <c r="DM28" s="126"/>
       <c r="DN28" s="83"/>
       <c r="DO28" s="83"/>
@@ -37149,11 +37107,9 @@
       <c r="DJ29" s="137"/>
       <c r="DK29" s="91" t="str">
         <f>W49</f>
-        <v>Belgia</v>
-      </c>
-      <c r="DL29" s="59">
-        <v>1</v>
-      </c>
+        <v>V43</v>
+      </c>
+      <c r="DL29" s="59"/>
       <c r="DM29" s="127"/>
       <c r="DN29" s="86"/>
       <c r="DO29" s="83"/>
@@ -37427,11 +37383,9 @@
       </c>
       <c r="DE30" s="90" t="str">
         <f>BC32</f>
-        <v>Belgia</v>
-      </c>
-      <c r="DF30" s="61">
-        <v>2</v>
-      </c>
+        <v>1E</v>
+      </c>
+      <c r="DF30" s="61"/>
       <c r="DG30" s="126"/>
       <c r="DH30" s="87"/>
       <c r="DI30" s="83"/>
@@ -37579,9 +37533,7 @@
         <f>BC27</f>
         <v>Tsjekkisk Republikk</v>
       </c>
-      <c r="DF31" s="59">
-        <v>0</v>
-      </c>
+      <c r="DF31" s="59"/>
       <c r="DG31" s="127"/>
       <c r="DH31" s="83"/>
       <c r="DI31" s="83"/>
@@ -37735,7 +37687,7 @@
       </c>
       <c r="AM32" s="116">
         <f>DA32</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN32" s="117" t="str">
         <f>INDEX(T,67,lang)</f>
@@ -37743,7 +37695,7 @@
       </c>
       <c r="AO32" s="116">
         <f>COUNTIF($V$7:$W$42,"=" &amp; AN32 &amp; "_win")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AP32" s="116">
         <f>COUNTIF($V$7:$W$42,"=" &amp; AN32 &amp; "_draw")</f>
@@ -37755,7 +37707,7 @@
       </c>
       <c r="AR32" s="116">
         <f>SUMIF($E$10:$E$45,$AN32,$F$10:$F$45) + SUMIF($H$10:$H$45,$AN32,$G$10:$G$45)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AS32" s="116">
         <f>SUMIF($E$10:$E$45,$AN32,$G$10:$G$45) + SUMIF($H$10:$H$45,$AN32,$F$10:$F$45)</f>
@@ -37763,23 +37715,23 @@
       </c>
       <c r="AT32" s="116">
         <f>AW32*10000</f>
-        <v>70000</v>
+        <v>40000</v>
       </c>
       <c r="AU32" s="116">
         <f>AR32-AS32</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AV32" s="116">
         <f>(AU32-AU37)/AU36</f>
-        <v>0.91666666666666663</v>
+        <v>0.9</v>
       </c>
       <c r="AW32" s="116">
         <f>AO32*3+AP32</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AX32" s="116">
         <f>BD32/BD36*10+BE32/BE36+BH32/BH36*0.1+BF32/BF36*0.01</f>
-        <v>0.505</v>
+        <v>0</v>
       </c>
       <c r="BA32" s="116">
         <f>VLOOKUP(AN32,db_fifarank,2,FALSE)/2000000</f>
@@ -37787,11 +37739,11 @@
       </c>
       <c r="BB32" s="117">
         <f>10000000*AW32/AW36+100000*AX32/AX36+100*AV32+10*AR32/AR36+1*AX32/AX36+BA32</f>
-        <v>8783656.8367115874</v>
+        <v>5000098.017221</v>
       </c>
       <c r="BC32" s="117" t="str">
         <f>IF(SUM(AO32:AQ35)=12,M33,INDEX(T,78,lang))</f>
-        <v>Belgia</v>
+        <v>1E</v>
       </c>
       <c r="BD32" s="116">
         <f>SUMPRODUCT(($V$7:$V$42=AN32&amp;"_win")*($X$7:$X$42))+SUMPRODUCT(($W$7:$W$42=AN32&amp;"_win")*($X$7:$X$42))</f>
@@ -37799,15 +37751,15 @@
       </c>
       <c r="BE32" s="121">
         <f>SUMPRODUCT(($V$7:$V$42=AN32&amp;"_draw")*($X$7:$X$42))+SUMPRODUCT(($W$7:$W$42=AN32&amp;"_draw")*($X$7:$X$42))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF32" s="121">
         <f>SUMPRODUCT(($E$10:$E$45=AN32)*($X$7:$X$42)*($F$10:$F$45))+SUMPRODUCT(($H$10:$H$45=AN32)*($X$7:$X$42)*($G$10:$G$45))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG32" s="121">
         <f>SUMPRODUCT(($E$10:$E$45=AN32)*($X$7:$X$42)*($G$10:$G$45))+SUMPRODUCT(($H$10:$H$45=AN32)*($X$7:$X$42)*($F$10:$F$45))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH32" s="121">
         <f>BF32-BG32</f>
@@ -37823,11 +37775,11 @@
       </c>
       <c r="BP32" s="121">
         <f>IFERROR(VLOOKUP("514",$AD$7:$AG$42,2,FALSE),0) + IFERROR(VLOOKUP("514",$AH$7:$AK$42,2,FALSE),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BQ32" s="122">
         <f>SUM(BM32:BP32)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BS32" s="121">
         <f>IFERROR(VLOOKUP("512",$AD$7:$AG$42,3,FALSE),0) + IFERROR(VLOOKUP("512",$AH$7:$AK$42,3,FALSE),0)</f>
@@ -37839,11 +37791,11 @@
       </c>
       <c r="BU32" s="121">
         <f>IFERROR(VLOOKUP("514",$AD$7:$AG$42,3,FALSE),0) + IFERROR(VLOOKUP("514",$AH$7:$AK$42,3,FALSE),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="BV32" s="122">
         <f>SUM(BR32:BU32)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="BW32" s="122">
         <f>RANK(BV32,BV32:BV35)</f>
@@ -37859,11 +37811,11 @@
       </c>
       <c r="CA32" s="121">
         <f>IFERROR(VLOOKUP("514",$AD$7:$AG$42,4,FALSE),0) + IFERROR(VLOOKUP("514",$AH$7:$AK$42,4,FALSE),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="CB32" s="122">
         <f>SUM(BX32:CA32)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="CD32" s="121">
         <f>IF(BN36=BQ32,BN32,0)</f>
@@ -37871,7 +37823,7 @@
       </c>
       <c r="CE32" s="121">
         <f>IF(BO36=BQ32,BO32,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CF32" s="121">
         <f>IF(BP36=BQ32,BP32,0)</f>
@@ -37879,7 +37831,7 @@
       </c>
       <c r="CG32" s="122">
         <f>SUM(CC32:CF32)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CI32" s="121">
         <f>IF(BN36=BQ32,BS32,0)</f>
@@ -37907,7 +37859,7 @@
       </c>
       <c r="CP32" s="121">
         <f>IF(BO36=BQ32,BZ32,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CQ32" s="121">
         <f>IF(BP36=BQ32,CA32,0)</f>
@@ -37915,15 +37867,15 @@
       </c>
       <c r="CR32" s="122">
         <f>SUM(CN32:CQ32)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CS32" s="122">
         <f>BQ32*10000+CG32*100+(5-CM32)+CR32/10</f>
-        <v>70104.100000000006</v>
+        <v>50004</v>
       </c>
       <c r="CT32" s="122">
         <f>RANK(CS32,CS32:CS35)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CV32" s="121">
         <f>IF(CV36=CT32,BN32,0)</f>
@@ -37931,7 +37883,7 @@
       </c>
       <c r="CW32" s="121">
         <f>IF(CW36=CT32,BO32,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CX32" s="121">
         <f>IF(CX36=CT32,BP32,0)</f>
@@ -37939,15 +37891,15 @@
       </c>
       <c r="CY32" s="122">
         <f>SUM(CU32:CX32)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CZ32" s="122">
         <f>(5-CT32)*10000+CY32*100+(5-BW32)+CB32/10+BA32/100</f>
-        <v>40104.600172209997</v>
+        <v>30004.40017221</v>
       </c>
       <c r="DA32" s="122">
         <f>RANK(CZ32,CZ32:CZ35)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DD32" s="120"/>
       <c r="DE32" s="83"/>
@@ -37966,11 +37918,9 @@
       </c>
       <c r="DQ32" s="90" t="str">
         <f>W59</f>
-        <v>Tyskland</v>
-      </c>
-      <c r="DR32" s="61">
-        <v>2</v>
-      </c>
+        <v>V47</v>
+      </c>
+      <c r="DR32" s="61"/>
       <c r="DS32" s="126"/>
       <c r="DT32" s="87"/>
       <c r="DU32" s="88"/>
@@ -38013,7 +37963,7 @@
       <c r="K33" s="145"/>
       <c r="M33" s="22" t="str">
         <f>VLOOKUP(1,AM32:AW35,2,FALSE)</f>
-        <v>Belgia</v>
+        <v>Italia</v>
       </c>
       <c r="N33" s="27">
         <f>O33+P33+Q33</f>
@@ -38033,7 +37983,7 @@
       </c>
       <c r="R33" s="27" t="str">
         <f>VLOOKUP(1,AM32:AW35,6,FALSE) &amp; " - " &amp; VLOOKUP(1,AM32:AW35,7,FALSE)</f>
-        <v>6 - 1</v>
+        <v>5 - 2</v>
       </c>
       <c r="S33" s="28">
         <f>O33*3+P33</f>
@@ -38161,11 +38111,11 @@
       </c>
       <c r="BB33" s="117">
         <f>10000000*AW33/AW36+100000*AX33/AX36+100*AV33+10*AR33/AR36+1*AX33/AX36+BA33</f>
-        <v>1.6801176666666668</v>
+        <v>2.0134509999999999</v>
       </c>
       <c r="BC33" s="117" t="str">
         <f>IF(SUM(AO32:AQ35)=12,M34,INDEX(T,79,lang))</f>
-        <v>Italia</v>
+        <v>2E</v>
       </c>
       <c r="BD33" s="116">
         <f>SUMPRODUCT(($V$7:$V$42=AN33&amp;"_win")*($X$7:$X$42))+SUMPRODUCT(($W$7:$W$42=AN33&amp;"_win")*($X$7:$X$42))</f>
@@ -38341,11 +38291,9 @@
       <c r="DP33" s="137"/>
       <c r="DQ33" s="91" t="str">
         <f>W60</f>
-        <v>Frankrike</v>
-      </c>
-      <c r="DR33" s="59">
-        <v>1</v>
-      </c>
+        <v>V48</v>
+      </c>
+      <c r="DR33" s="59"/>
       <c r="DS33" s="127"/>
       <c r="DT33" s="88"/>
       <c r="DU33" s="88"/>
@@ -38388,15 +38336,15 @@
       <c r="K34" s="145"/>
       <c r="M34" s="23" t="str">
         <f>VLOOKUP(2,AM32:AW35,2,FALSE)</f>
-        <v>Italia</v>
+        <v>Belgia</v>
       </c>
       <c r="N34" s="29">
         <f>O34+P34+Q34</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O34" s="29">
         <f>VLOOKUP(2,AM32:AW35,3,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P34" s="29">
         <f>VLOOKUP(2,AM32:AW35,4,FALSE)</f>
@@ -38408,11 +38356,11 @@
       </c>
       <c r="R34" s="29" t="str">
         <f>VLOOKUP(2,AM32:AW35,6,FALSE) &amp; " - " &amp; VLOOKUP(2,AM32:AW35,7,FALSE)</f>
-        <v>5 - 2</v>
+        <v>4 - 1</v>
       </c>
       <c r="S34" s="30">
         <f>O34*3+P34</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="U34" s="116">
         <f>DATE(2016,6,20)+TIME(8,0,0)+gmt_delta</f>
@@ -38484,7 +38432,7 @@
       </c>
       <c r="AM34" s="116">
         <f t="shared" si="46"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN34" s="117" t="str">
         <f>INDEX(T,41,lang)</f>
@@ -38520,7 +38468,7 @@
       </c>
       <c r="AV34" s="116">
         <f>(AU34-AU37)/AU36</f>
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="AW34" s="116">
         <f>AO34*3+AP34</f>
@@ -38528,7 +38476,7 @@
       </c>
       <c r="AX34" s="116">
         <f>BD34/BD36*10+BE34/BE36+BH34/BH36*0.1+BF34/BF36*0.01</f>
-        <v>0.505</v>
+        <v>0</v>
       </c>
       <c r="BA34" s="116">
         <f>VLOOKUP(AN34,db_fifarank,2,FALSE)/2000000</f>
@@ -38536,7 +38484,7 @@
       </c>
       <c r="BB34" s="117">
         <f>10000000*AW34/AW36+100000*AX34/AX36+100*AV34+10*AR34/AR36+1*AX34/AX36+BA34</f>
-        <v>8783638.5033297557</v>
+        <v>8750100.0171725005</v>
       </c>
       <c r="BC34" s="117" t="str">
         <f>IF(SUM(AO32:AQ35)&gt;0,M35,"3E")</f>
@@ -38548,15 +38496,15 @@
       </c>
       <c r="BE34" s="121">
         <f>SUMPRODUCT(($V$7:$V$42=AN34&amp;"_draw")*($X$7:$X$42))+SUMPRODUCT(($W$7:$W$42=AN34&amp;"_draw")*($X$7:$X$42))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF34" s="121">
         <f>SUMPRODUCT(($E$10:$E$45=AN34)*($X$7:$X$42)*($F$10:$F$45))+SUMPRODUCT(($H$10:$H$45=AN34)*($X$7:$X$42)*($G$10:$G$45))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BG34" s="121">
         <f>SUMPRODUCT(($E$10:$E$45=AN34)*($X$7:$X$42)*($G$10:$G$45))+SUMPRODUCT(($H$10:$H$45=AN34)*($X$7:$X$42)*($F$10:$F$45))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH34" s="121">
         <f>BF34-BG34</f>
@@ -38596,7 +38544,7 @@
       </c>
       <c r="BW34" s="122">
         <f>RANK(BV34,BV32:BV35)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BX34" s="121">
         <f>IFERROR(VLOOKUP("531",$AD$7:$AG$42,4,FALSE),0) + IFERROR(VLOOKUP("531",$AH$7:$AK$42,4,FALSE),0)</f>
@@ -38616,7 +38564,7 @@
       </c>
       <c r="CC34" s="121">
         <f>IF(BM36=BQ34,BM34,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD34" s="121">
         <f>IF(BN36=BQ34,BN34,0)</f>
@@ -38628,7 +38576,7 @@
       </c>
       <c r="CG34" s="122">
         <f>SUM(CC34:CF34)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CH34" s="121">
         <f>IF(BM36=BQ34,BR34,0)</f>
@@ -38652,7 +38600,7 @@
       </c>
       <c r="CN34" s="121">
         <f>IF(BM36=BQ34,BX34,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CO34" s="121">
         <f>IF(BN36=BQ34,BY34,0)</f>
@@ -38664,11 +38612,11 @@
       </c>
       <c r="CR34" s="122">
         <f>SUM(CN34:CQ34)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CS34" s="122">
         <f t="shared" si="47"/>
-        <v>70104.100000000006</v>
+        <v>70004</v>
       </c>
       <c r="CT34" s="122">
         <f>RANK(CS34,CS32:CS35)</f>
@@ -38676,7 +38624,7 @@
       </c>
       <c r="CU34" s="121">
         <f>IF(CU36=CT34,BM34,0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CV34" s="121">
         <f>IF(CV36=CT34,BN34,0)</f>
@@ -38688,15 +38636,15 @@
       </c>
       <c r="CY34" s="122">
         <f t="shared" si="48"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CZ34" s="122">
         <f t="shared" si="49"/>
-        <v>40103.500171724998</v>
+        <v>40004.500171724998</v>
       </c>
       <c r="DA34" s="122">
         <f>RANK(CZ34,CZ32:CZ35)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DD34" s="138">
         <v>40</v>
@@ -38705,9 +38653,7 @@
         <f>BC8</f>
         <v>Frankrike</v>
       </c>
-      <c r="DF34" s="61">
-        <v>2</v>
-      </c>
+      <c r="DF34" s="61"/>
       <c r="DG34" s="126"/>
       <c r="DH34" s="83"/>
       <c r="DI34" s="83"/>
@@ -38766,7 +38712,7 @@
       </c>
       <c r="N35" s="29">
         <f>O35+P35+Q35</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O35" s="29">
         <f>VLOOKUP(3,AM32:AW35,3,FALSE)</f>
@@ -38778,11 +38724,11 @@
       </c>
       <c r="Q35" s="29">
         <f>VLOOKUP(3,AM32:AW35,5,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R35" s="29" t="str">
         <f>VLOOKUP(3,AM32:AW35,6,FALSE) &amp; " - " &amp; VLOOKUP(3,AM32:AW35,7,FALSE)</f>
-        <v>1 - 3</v>
+        <v>1 - 1</v>
       </c>
       <c r="S35" s="30">
         <f>O35*3+P35</f>
@@ -38874,7 +38820,7 @@
       </c>
       <c r="AQ35" s="116">
         <f>COUNTIF($V$7:$W$42,"=" &amp; AN35 &amp; "_lose")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR35" s="116">
         <f>SUMIF($E$10:$E$45,$AN35,$F$10:$F$45) + SUMIF($H$10:$H$45,$AN35,$G$10:$G$45)</f>
@@ -38882,7 +38828,7 @@
       </c>
       <c r="AS35" s="116">
         <f>SUMIF($E$10:$E$45,$AN35,$G$10:$G$45) + SUMIF($H$10:$H$45,$AN35,$F$10:$F$45)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AT35" s="116">
         <f>AW35*10000</f>
@@ -38890,11 +38836,11 @@
       </c>
       <c r="AU35" s="116">
         <f>AR35-AS35</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AV35" s="116">
         <f>(AU35-AU37)/AU36</f>
-        <v>0.33333333333333331</v>
+        <v>0.6</v>
       </c>
       <c r="AW35" s="116">
         <f>AO35*3+AP35</f>
@@ -38910,7 +38856,7 @@
       </c>
       <c r="BB35" s="117">
         <f>10000000*AW35/AW36+100000*AX35/AX36+100*AV35+10*AR35/AR36+1*AX35/AX36+BA35</f>
-        <v>3750035.0145140002</v>
+        <v>3750062.0145140002</v>
       </c>
       <c r="BD35" s="116">
         <f>SUMPRODUCT(($V$7:$V$42=AN35&amp;"_win")*($X$7:$X$42))+SUMPRODUCT(($W$7:$W$42=AN35&amp;"_win")*($X$7:$X$42))</f>
@@ -38934,7 +38880,7 @@
       </c>
       <c r="BM35" s="121">
         <f>IFERROR(VLOOKUP("541",$AD$7:$AG$42,2,FALSE),0) + IFERROR(VLOOKUP("541",$AH$7:$AK$42,2,FALSE),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN35" s="121">
         <f>IFERROR(VLOOKUP("542",$AD$7:$AG$42,2,FALSE),0) + IFERROR(VLOOKUP("542",$AH$7:$AK$42,2,FALSE),0)</f>
@@ -38946,11 +38892,11 @@
       </c>
       <c r="BQ35" s="122">
         <f>SUM(BM35:BP35)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BR35" s="121">
         <f>IFERROR(VLOOKUP("541",$AD$7:$AG$42,3,FALSE),0) + IFERROR(VLOOKUP("541",$AH$7:$AK$42,3,FALSE),0)</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="BS35" s="121">
         <f>IFERROR(VLOOKUP("542",$AD$7:$AG$42,3,FALSE),0) + IFERROR(VLOOKUP("542",$AH$7:$AK$42,3,FALSE),0)</f>
@@ -38962,7 +38908,7 @@
       </c>
       <c r="BV35" s="122">
         <f>SUM(BR35:BU35)</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="BW35" s="122">
         <f>RANK(BV35,BV32:BV35)</f>
@@ -39038,7 +38984,7 @@
       </c>
       <c r="CS35" s="122">
         <f t="shared" si="47"/>
-        <v>30004</v>
+        <v>40004</v>
       </c>
       <c r="CT35" s="122">
         <f>RANK(CS35,CS32:CS35)</f>
@@ -39073,9 +39019,7 @@
         <f>VLOOKUP(lookup_3rd, tbl_lookup_3rd,2,FALSE)</f>
         <v>Ukraina</v>
       </c>
-      <c r="DF35" s="59">
-        <v>0</v>
-      </c>
+      <c r="DF35" s="59"/>
       <c r="DG35" s="127"/>
       <c r="DH35" s="86"/>
       <c r="DI35" s="83"/>
@@ -39241,7 +39185,7 @@
       </c>
       <c r="AR36" s="116">
         <f t="shared" si="50"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AS36" s="116">
         <f t="shared" si="50"/>
@@ -39253,7 +39197,7 @@
       </c>
       <c r="AU36" s="116">
         <f>MAX(AU32:AU35)-AU37+1</f>
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AW36" s="116">
         <f t="shared" si="50"/>
@@ -39261,7 +39205,7 @@
       </c>
       <c r="AX36" s="116">
         <f t="shared" si="50"/>
-        <v>1.5049999999999999</v>
+        <v>1</v>
       </c>
       <c r="BD36" s="116">
         <f>MAX(BD32:BD35)-MIN(BD32:BD35)+1</f>
@@ -39269,15 +39213,15 @@
       </c>
       <c r="BE36" s="116">
         <f>MAX(BE32:BE35)-MIN(BE32:BE35)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BF36" s="116">
         <f>MAX(BF32:BF35)-MIN(BF32:BF35)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BG36" s="116">
         <f>MAX(BG32:BG35)-MIN(BG32:BG35)+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="BH36" s="116">
         <f>MAX(BH32:BH35)-MIN(BH32:BH35)+1</f>
@@ -39285,7 +39229,7 @@
       </c>
       <c r="BM36" s="116">
         <f>BQ32</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="BN36" s="116">
         <f>BQ33</f>
@@ -39297,7 +39241,7 @@
       </c>
       <c r="BP36" s="116">
         <f>BQ35</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="BR36" s="116"/>
       <c r="BS36" s="116"/>
@@ -39321,7 +39265,7 @@
       <c r="CQ36" s="116"/>
       <c r="CU36" s="116">
         <f>CT32</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="CV36" s="116">
         <f>CT33</f>
@@ -39337,7 +39281,7 @@
       </c>
       <c r="CY36" s="122">
         <f t="shared" si="48"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="DD36" s="120"/>
       <c r="DE36" s="83"/>
@@ -39350,11 +39294,9 @@
       </c>
       <c r="DK36" s="90" t="str">
         <f>W52</f>
-        <v>Frankrike</v>
-      </c>
-      <c r="DL36" s="61">
-        <v>3</v>
-      </c>
+        <v>V40</v>
+      </c>
+      <c r="DL36" s="61"/>
       <c r="DM36" s="126"/>
       <c r="DN36" s="87"/>
       <c r="DO36" s="83"/>
@@ -39489,11 +39431,9 @@
       <c r="DJ37" s="137"/>
       <c r="DK37" s="91" t="str">
         <f>W53</f>
-        <v>Island</v>
-      </c>
-      <c r="DL37" s="59">
-        <v>1</v>
-      </c>
+        <v>V44</v>
+      </c>
+      <c r="DL37" s="59"/>
       <c r="DM37" s="127"/>
       <c r="DN37" s="83"/>
       <c r="DO37" s="83"/>
@@ -39863,12 +39803,8 @@
         <f>BC15</f>
         <v>Russland</v>
       </c>
-      <c r="DF38" s="61">
-        <v>1</v>
-      </c>
-      <c r="DG38" s="126">
-        <v>5</v>
-      </c>
+      <c r="DF38" s="61"/>
+      <c r="DG38" s="126"/>
       <c r="DH38" s="87"/>
       <c r="DI38" s="83"/>
       <c r="DN38" s="83"/>
@@ -40237,12 +40173,8 @@
         <f>BC39</f>
         <v>Island</v>
       </c>
-      <c r="DF39" s="59">
-        <v>1</v>
-      </c>
-      <c r="DG39" s="127">
-        <v>6</v>
-      </c>
+      <c r="DF39" s="59"/>
+      <c r="DG39" s="127"/>
       <c r="DH39" s="83"/>
       <c r="DI39" s="83"/>
       <c r="DP39" s="83"/>
@@ -40959,7 +40891,7 @@
       <c r="DS41" s="154"/>
       <c r="DT41" s="156" t="str">
         <f>V73</f>
-        <v>Tyskland</v>
+        <v/>
       </c>
       <c r="DU41" s="156"/>
       <c r="DV41" s="156"/>
@@ -41037,11 +40969,11 @@
       </c>
       <c r="V42" s="118" t="str">
         <f t="shared" si="0"/>
-        <v>Sverige_lose</v>
+        <v/>
       </c>
       <c r="W42" s="118" t="str">
         <f t="shared" si="1"/>
-        <v>Belgia_win</v>
+        <v/>
       </c>
       <c r="X42" s="117">
         <f t="shared" si="2"/>
@@ -41073,11 +41005,11 @@
       </c>
       <c r="AE42" s="116">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF42" s="116">
         <f t="shared" si="10"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AG42" s="116">
         <f t="shared" si="11"/>
@@ -41089,15 +41021,15 @@
       </c>
       <c r="AI42" s="116">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AJ42" s="116">
         <f t="shared" si="13"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK42" s="116">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO42" s="116">
         <f t="shared" ref="AO42:AX42" si="55">MAX(AO38:AO41)-MIN(AO38:AO41)+1</f>
@@ -41405,12 +41337,8 @@
         <f>AN35</f>
         <v>Sverige</v>
       </c>
-      <c r="F45" s="59">
-        <v>0</v>
-      </c>
-      <c r="G45" s="60">
-        <v>2</v>
-      </c>
+      <c r="F45" s="59"/>
+      <c r="G45" s="60"/>
       <c r="H45" s="82" t="str">
         <f>AN32</f>
         <v>Belgia</v>
@@ -41509,7 +41437,7 @@
       </c>
       <c r="N46" s="29">
         <f t="shared" ref="N46:N50" si="64">O46+P46+Q46</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O46" s="29">
         <f>VLOOKUP(2,AM44:AW49,3,FALSE)</f>
@@ -41521,11 +41449,11 @@
       </c>
       <c r="Q46" s="29">
         <f>VLOOKUP(2,AM44:AW49,5,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R46" s="29" t="str">
         <f>VLOOKUP(2,AM44:AW49,6,FALSE) &amp; " - " &amp; VLOOKUP(2,AM44:AW49,7,FALSE)</f>
-        <v>1 - 3</v>
+        <v>1 - 1</v>
       </c>
       <c r="S46" s="30">
         <f t="shared" ref="S46:S50" si="65">O46*3+P46</f>
@@ -41537,11 +41465,11 @@
       </c>
       <c r="V46" s="118" t="str">
         <f>IF(OR(DF10="",DF11=""),"",IF(DF10&gt;DF11,DE10,IF(DF10&lt;DF11,DE11,IF(OR(DG10="",DG11=""),"draw",IF(DG10&gt;DG11,DE10,IF(DG10&lt;DG11,DE11,"draw"))))))</f>
-        <v>Sveits</v>
+        <v/>
       </c>
       <c r="W46" s="118" t="str">
         <f>IF(OR(V46="",V46="draw"),INDEX(T,86,lang),V46)</f>
-        <v>Sveits</v>
+        <v>V37</v>
       </c>
       <c r="AL46" s="117" t="str">
         <f>IF(AM46&lt;5,"C","")</f>
@@ -41631,11 +41559,11 @@
       </c>
       <c r="V47" s="118" t="str">
         <f>IF(OR(DF14="",DF15=""),"",IF(DF14&gt;DF15,DE14,IF(DF14&lt;DF15,DE15,IF(OR(DG14="",DG15=""),"draw",IF(DG14&gt;DG15,DE14,IF(DG14&lt;DG15,DE15,"draw"))))))</f>
-        <v>Spania</v>
+        <v/>
       </c>
       <c r="W47" s="118" t="str">
         <f>IF(OR(V47="",V47="draw"),INDEX(T,87,lang),V47)</f>
-        <v>Spania</v>
+        <v>V39</v>
       </c>
       <c r="AL47" s="117" t="str">
         <f>IF(AM47&lt;5,"D","")</f>
@@ -41725,11 +41653,11 @@
       </c>
       <c r="V48" s="118" t="str">
         <f>IF(OR(DF26="",DF27=""),"",IF(DF26&gt;DF27,DE26,IF(DF26&lt;DF27,DE27,IF(OR(DG26="",DG27=""),"draw",IF(DG26&gt;DG27,DE26,IF(DG26&lt;DG27,DE27,"draw"))))))</f>
-        <v>Tyskland</v>
+        <v/>
       </c>
       <c r="W48" s="118" t="str">
         <f>IF(OR(V48="",V48="draw"),INDEX(T,88,lang),V48)</f>
-        <v>Tyskland</v>
+        <v>V41</v>
       </c>
       <c r="AL48" s="117" t="str">
         <f>IF(AM48&lt;5,"E","")</f>
@@ -41753,7 +41681,7 @@
       </c>
       <c r="AQ48" s="116">
         <f t="shared" si="57"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR48" s="116">
         <f t="shared" si="58"/>
@@ -41761,15 +41689,15 @@
       </c>
       <c r="AS48" s="116">
         <f t="shared" si="59"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AU48" s="116">
         <f t="shared" si="61"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="AV48" s="116">
         <f>(AU48-AU51)/AU50</f>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="AW48" s="116">
         <f t="shared" si="62"/>
@@ -41781,7 +41709,7 @@
       </c>
       <c r="BB48" s="117">
         <f t="shared" si="63"/>
-        <v>7925.0145140000004</v>
+        <v>8325.0145140000004</v>
       </c>
       <c r="BE48" s="116"/>
       <c r="BF48" s="116"/>
@@ -41851,11 +41779,11 @@
       </c>
       <c r="V49" s="118" t="str">
         <f>IF(OR(DF30="",DF31=""),"",IF(DF30&gt;DF31,DE30,IF(DF30&lt;DF31,DE31,IF(OR(DG30="",DG31=""),"draw",IF(DG30&gt;DG31,DE30,IF(DG30&lt;DG31,DE31,"draw"))))))</f>
-        <v>Belgia</v>
+        <v/>
       </c>
       <c r="W49" s="118" t="str">
         <f>IF(OR(V49="",V49="draw"),INDEX(T,89,lang),V49)</f>
-        <v>Belgia</v>
+        <v>V43</v>
       </c>
       <c r="AL49" s="117" t="str">
         <f>IF(AM49&lt;5,"F","")</f>
@@ -41945,11 +41873,11 @@
       </c>
       <c r="V50" s="118" t="str">
         <f>IF(OR(DF18="",DF19=""),"",IF(DF18&gt;DF19,DE18,IF(DF18&lt;DF19,DE19,IF(OR(DG18="",DG19=""),"draw",IF(DG18&gt;DG19,DE18,IF(DG18&lt;DG19,DE19,"draw"))))))</f>
-        <v>England</v>
+        <v/>
       </c>
       <c r="W50" s="118" t="str">
         <f>IF(OR(V50="",V50="draw"),INDEX(T,90,lang),V50)</f>
-        <v>England</v>
+        <v>V38</v>
       </c>
       <c r="AL50" s="117" t="str">
         <f>AL44&amp;AL45&amp;AL46&amp;AL47&amp;AL48&amp;AL49</f>
@@ -41973,7 +41901,7 @@
       </c>
       <c r="AS50" s="116">
         <f>MAX(AS44:AS49)-MIN(AS44:AS49)+1</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AU50" s="116">
         <f>MAX(AU44:AU49)-AU51+1</f>
@@ -41992,11 +41920,11 @@
       </c>
       <c r="V51" s="118" t="str">
         <f>IF(OR(DF22="",DF23=""),"",IF(DF22&gt;DF23,DE22,IF(DF22&lt;DF23,DE23,IF(OR(DG22="",DG23=""),"draw",IF(DG22&gt;DG23,DE22,IF(DG22&lt;DG23,DE23,"draw"))))))</f>
-        <v>Italia</v>
+        <v/>
       </c>
       <c r="W51" s="118" t="str">
         <f>IF(OR(V51="",V51="draw"),INDEX(T,91,lang),V51)</f>
-        <v>Italia</v>
+        <v>V42</v>
       </c>
       <c r="AU51" s="116">
         <f>MIN(AU44:AU49)</f>
@@ -42034,11 +41962,11 @@
       </c>
       <c r="V52" s="118" t="str">
         <f>IF(OR(DF34="",DF35=""),"",IF(DF34&gt;DF35,DE34,IF(DF34&lt;DF35,DE35,IF(OR(DG34="",DG35=""),"draw",IF(DG34&gt;DG35,DE34,IF(DG34&lt;DG35,DE35,"draw"))))))</f>
-        <v>Frankrike</v>
+        <v/>
       </c>
       <c r="W52" s="118" t="str">
         <f>IF(OR(V52="",V52="draw"),INDEX(T,92,lang),V52)</f>
-        <v>Frankrike</v>
+        <v>V40</v>
       </c>
       <c r="BA52" s="116"/>
     </row>
@@ -42066,11 +41994,11 @@
       </c>
       <c r="V53" s="118" t="str">
         <f>IF(OR(DF38="",DF39=""),"",IF(DF38&gt;DF39,DE38,IF(DF38&lt;DF39,DE39,IF(OR(DG38="",DG39=""),"draw",IF(DG38&gt;DG39,DE38,IF(DG38&lt;DG39,DE39,"draw"))))))</f>
-        <v>Island</v>
+        <v/>
       </c>
       <c r="W53" s="118" t="str">
         <f>IF(OR(V53="",V53="draw"),INDEX(T,93,lang),V53)</f>
-        <v>Island</v>
+        <v>V44</v>
       </c>
       <c r="AN53" s="124" t="s">
         <v>1708</v>
@@ -42246,11 +42174,11 @@
       </c>
       <c r="V57" s="118" t="str">
         <f>IF(OR(DL12="",DL13=""),"",IF(DL12&gt;DL13,DK12,IF(DL12&lt;DL13,DK13,IF(OR(DM12="",DM13=""),"draw",IF(DM12&gt;DM13,DK12,IF(DM12&lt;DM13,DK13,"draw"))))))</f>
-        <v>Spania</v>
+        <v/>
       </c>
       <c r="W57" s="118" t="str">
         <f>IF(OR(V57="",V57="draw"),INDEX(T,94,lang),V57)</f>
-        <v>Spania</v>
+        <v>V45</v>
       </c>
       <c r="AN57" s="124" t="s">
         <v>1712</v>
@@ -42291,11 +42219,11 @@
       </c>
       <c r="V58" s="118" t="str">
         <f>IF(OR(DL20="",DL21=""),"",IF(DL20&gt;DL21,DK20,IF(DL20&lt;DL21,DK21,IF(OR(DM20="",DM21=""),"draw",IF(DM20&gt;DM21,DK20,IF(DM20&lt;DM21,DK21,"draw"))))))</f>
-        <v>Italia</v>
+        <v/>
       </c>
       <c r="W58" s="118" t="str">
         <f>IF(OR(V58="",V58="draw"),INDEX(T,95,lang),V58)</f>
-        <v>Italia</v>
+        <v>V46</v>
       </c>
       <c r="AN58" s="124" t="s">
         <v>1713</v>
@@ -42336,11 +42264,11 @@
       </c>
       <c r="V59" s="118" t="str">
         <f>IF(OR(DL28="",DL29=""),"",IF(DL28&gt;DL29,DK28,IF(DL28&lt;DL29,DK29,IF(OR(DM28="",DM29=""),"draw",IF(DM28&gt;DM29,DK28,IF(DM28&lt;DM29,DK29,"draw"))))))</f>
-        <v>Tyskland</v>
+        <v/>
       </c>
       <c r="W59" s="118" t="str">
         <f>IF(OR(V59="",V59="draw"),INDEX(T,96,lang),V59)</f>
-        <v>Tyskland</v>
+        <v>V47</v>
       </c>
       <c r="AN59" s="124" t="s">
         <v>1714</v>
@@ -42381,11 +42309,11 @@
       </c>
       <c r="V60" s="118" t="str">
         <f>IF(OR(DL36="",DL37=""),"",IF(DL36&gt;DL37,DK36,IF(DL36&lt;DL37,DK37,IF(OR(DM36="",DM37=""),"draw",IF(DM36&gt;DM37,DK36,IF(DM36&lt;DM37,DK37,"draw"))))))</f>
-        <v>Frankrike</v>
+        <v/>
       </c>
       <c r="W60" s="118" t="str">
         <f>IF(OR(V60="",V60="draw"),INDEX(T,97,lang),V60)</f>
-        <v>Frankrike</v>
+        <v>V48</v>
       </c>
       <c r="AN60" s="124" t="s">
         <v>1715</v>
@@ -42525,15 +42453,15 @@
       </c>
       <c r="V64" s="118" t="str">
         <f>IF(OR(DR16="",DR17=""),"",IF(DR16&gt;DR17,DQ16,IF(DR16&lt;DR17,DQ17,IF(OR(DS16="",DS17=""),"draw",IF(DS16&gt;DS17,DQ16,IF(DS16&lt;DS17,DQ17,"draw"))))))</f>
-        <v>Italia</v>
+        <v/>
       </c>
       <c r="W64" s="118" t="str">
         <f>IF(OR(V64="",V64="draw"),INDEX(T,98,lang),V64)</f>
-        <v>Italia</v>
+        <v>V49</v>
       </c>
       <c r="X64" s="118" t="str">
         <f>IF(OR(DR16="",DR17=""),"",IF(DR16&lt;DR17,DQ16,IF(DR16&gt;DR17,DQ17,IF(OR(DS16="",DS17=""),"draw",IF(DS16&lt;DS17,DQ16,IF(DS16&gt;DS17,DQ17,"draw"))))))</f>
-        <v>Spania</v>
+        <v/>
       </c>
       <c r="AN64" s="124" t="s">
         <v>1719</v>
@@ -42574,15 +42502,15 @@
       </c>
       <c r="V65" s="118" t="str">
         <f>IF(OR(DR32="",DR33=""),"",IF(DR32&gt;DR33,DQ32,IF(DR32&lt;DR33,DQ33,IF(OR(DS32="",DS33=""),"draw",IF(DS32&gt;DS33,DQ32,IF(DS32&lt;DS33,DQ33,"draw"))))))</f>
-        <v>Tyskland</v>
+        <v/>
       </c>
       <c r="W65" s="118" t="str">
         <f>IF(OR(V65="",V65="draw"),INDEX(T,99,lang),V65)</f>
-        <v>Tyskland</v>
+        <v>V50</v>
       </c>
       <c r="X65" s="118" t="str">
         <f>IF(OR(DR32="",DR33=""),"",IF(DR32&lt;DR33,DQ32,IF(DR32&gt;DR33,DQ33,IF(OR(DS32="",DS33=""),"draw",IF(DS32&lt;DS33,DQ32,IF(DS32&gt;DS33,DQ33,"draw"))))))</f>
-        <v>Frankrike</v>
+        <v/>
       </c>
       <c r="AN65" s="124" t="s">
         <v>1720</v>
@@ -42703,11 +42631,11 @@
       </c>
       <c r="V73" s="118" t="str">
         <f>IF(OR(DX23="",DX24=""),"",IF(DX23&gt;DX24,DW23,IF(DX23&lt;DX24,DW24,IF(OR(DY23="",DY24=""),"",IF(DY23&gt;DY24,DW23,IF(DY23&lt;DY24,DW24,""))))))</f>
-        <v>Tyskland</v>
+        <v/>
       </c>
       <c r="W73" s="118" t="str">
         <f>V73</f>
-        <v>Tyskland</v>
+        <v/>
       </c>
     </row>
     <row r="74" spans="21:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -42715,13 +42643,13 @@
     <row r="76" spans="21:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AL76" s="118" t="str">
         <f>IF(OR(X64="",X64="draw"),INDEX(T,100,lang),X64)</f>
-        <v>Spania</v>
+        <v>T61</v>
       </c>
     </row>
     <row r="77" spans="21:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AL77" s="118" t="str">
         <f>IF(OR(X65="",X65="draw"),INDEX(T,101,lang),X65)</f>
-        <v>Frankrike</v>
+        <v>T62</v>
       </c>
     </row>
     <row r="79" spans="21:48" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>